<commit_message>
almost done with question 2
</commit_message>
<xml_diff>
--- a/Lab 5/Lab 5.xlsx
+++ b/Lab 5/Lab 5.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prahershkumar/Documents/Prahersh Kumar/School /UIUC/Classes/Fall 2022/AE 460/AE-460/Lab 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5256170-6C35-B248-8DF1-4596A17790B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C3948-E256-C940-A829-DE22BF37BD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23920" yWindow="2760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{AB60D2C1-0B5B-2B40-AA37-C588C28FD481}"/>
+    <workbookView xWindow="5520" yWindow="3740" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{AB60D2C1-0B5B-2B40-AA37-C588C28FD481}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Question 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Question 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Querstion 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_2022_10_30_Sample_Data" localSheetId="0">Sheet1!$A$1:$L$1535</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Time (sec)</t>
   </si>
@@ -134,6 +135,45 @@
   <si>
     <t>Max</t>
   </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>h3</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>&amp; 383.5246</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;  946.4309 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp; 593.3661 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; 418.5055 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp; 1037.5250 </t>
+  </si>
+  <si>
+    <t>&amp; 605.2865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp; 452.7588 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp; 1119.5570 </t>
+  </si>
+  <si>
+    <t>&amp; 630.9921</t>
+  </si>
 </sst>
 </file>
 
@@ -174,8 +214,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10595,7 +10641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89748FBD-FF85-004A-B9FE-B732D65AA51D}">
   <dimension ref="A1:L1535"/>
   <sheetViews>
-    <sheetView topLeftCell="A1265" zoomScaleNormal="151" workbookViewId="0">
+    <sheetView zoomScaleNormal="151" workbookViewId="0">
       <selection activeCell="K1177" sqref="K1177"/>
     </sheetView>
   </sheetViews>
@@ -68952,8 +68998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07281655-9145-5741-9368-0DD2DF116671}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -69257,4 +69303,134 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A65B60A-661F-0F43-B3E3-27F4D90D7D8F}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>297.04989999999998</v>
+      </c>
+      <c r="C2">
+        <v>296.87959999999998</v>
+      </c>
+      <c r="D2">
+        <v>296.64589999999998</v>
+      </c>
+      <c r="E2">
+        <v>297.12779999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>48000</v>
+      </c>
+      <c r="B3">
+        <v>296.6773</v>
+      </c>
+      <c r="C3">
+        <v>326.75529999999998</v>
+      </c>
+      <c r="D3">
+        <v>806.72550000000001</v>
+      </c>
+      <c r="E3">
+        <v>475.95699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>58000</v>
+      </c>
+      <c r="B4">
+        <v>96.956800000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>68000</v>
+      </c>
+      <c r="B5">
+        <v>296.83449999999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>296.5224</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>